<commit_message>
Added in correct models for gears and mated everything accordingly.
</commit_message>
<xml_diff>
--- a/Hours_Expenses.xlsx
+++ b/Hours_Expenses.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bosleis\Documents\Stardust\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D14E451-7ADC-4106-A1CF-E99F0ADEB469}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7714B8-835C-43F8-92E9-EF6E5D919577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="3360" windowWidth="15240" windowHeight="11835" activeTab="1" xr2:uid="{7F05E2EB-2AD1-4C0C-AE0D-5436AF3ECC52}"/>
+    <workbookView xWindow="1410" yWindow="3360" windowWidth="15240" windowHeight="11835" activeTab="2" xr2:uid="{7F05E2EB-2AD1-4C0C-AE0D-5436AF3ECC52}"/>
   </bookViews>
   <sheets>
     <sheet name="Hours" sheetId="1" r:id="rId1"/>
     <sheet name="Expenses" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Date</t>
   </si>
@@ -73,6 +74,33 @@
   </si>
   <si>
     <t>Total Spent</t>
+  </si>
+  <si>
+    <t>Part Number</t>
+  </si>
+  <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>GPA18GT2060-A-H5</t>
+  </si>
+  <si>
+    <t>Item Name</t>
+  </si>
+  <si>
+    <t>MISUMI</t>
+  </si>
+  <si>
+    <t>GPA60GT2060-B-H8</t>
+  </si>
+  <si>
+    <t>GT2 Timing Belt Pulley 18 Tooth</t>
+  </si>
+  <si>
+    <t>GT2 Timing Belt Pulley 20 Tooth</t>
   </si>
 </sst>
 </file>
@@ -127,7 +155,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -135,6 +163,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -510,7 +539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D457D3EF-C0D0-4740-9C84-7FF3F6E5FFAE}">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -574,4 +603,66 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94508B3A-42B8-4A22-8CF8-052B895A670C}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="5">
+        <v>18.100000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="5">
+        <v>32.18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>